<commit_message>
T460 - miercuri 6 iulie 2022, 20:31:39 +0300
</commit_message>
<xml_diff>
--- a/SCRATCH/CLEAN/foaie_parcurs_B-151-VGT_iunie_2022_Alex_Bora.xlsx
+++ b/SCRATCH/CLEAN/foaie_parcurs_B-151-VGT_iunie_2022_Alex_Bora.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
   <si>
     <t>VOLVO ROMÂNIA</t>
   </si>
@@ -70,34 +70,37 @@
     <t>Observatii utilizator</t>
   </si>
   <si>
+    <t>Acasa-Birou</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Cluj-Dej</t>
+  </si>
+  <si>
+    <t>Interes Serviciu</t>
+  </si>
+  <si>
     <t>Cluj-Baia-Mare</t>
   </si>
   <si>
-    <t>Interes Serviciu</t>
+    <t>Cluj-Cmp. Turzii</t>
+  </si>
+  <si>
+    <t>Cluj-Turda</t>
+  </si>
+  <si>
+    <t>Cluj-Apahida</t>
+  </si>
+  <si>
+    <t>Cluj-Cluj</t>
   </si>
   <si>
     <t>Cluj-Bistrita</t>
   </si>
   <si>
-    <t>Cluj-Cmp. Turzii</t>
-  </si>
-  <si>
-    <t>Acasa-Birou</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Cluj-Bontida</t>
-  </si>
-  <si>
-    <t>Cluj-Apahida</t>
-  </si>
-  <si>
     <t>Cluj-Satu-Mare</t>
-  </si>
-  <si>
-    <t>Cluj-Turda</t>
   </si>
   <si>
     <t>Km parcursi:</t>
@@ -623,7 +626,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>238122</v>
+        <v>251008</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="20" customHeight="1">
@@ -655,7 +658,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="4">
-        <v>356</v>
+        <v>30</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>17</v>
@@ -669,13 +672,13 @@
         <v>3</v>
       </c>
       <c r="B16" s="4">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="20" customHeight="1">
@@ -703,13 +706,13 @@
         <v>6</v>
       </c>
       <c r="B19" s="4">
-        <v>152</v>
+        <v>356</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="20" customHeight="1">
@@ -717,13 +720,13 @@
         <v>7</v>
       </c>
       <c r="B20" s="4">
-        <v>30</v>
+        <v>152</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="20" customHeight="1">
@@ -731,10 +734,10 @@
         <v>8</v>
       </c>
       <c r="B21" s="4">
-        <v>92</v>
+        <v>30</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>18</v>
@@ -745,13 +748,13 @@
         <v>9</v>
       </c>
       <c r="B22" s="4">
-        <v>30</v>
+        <v>356</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="20" customHeight="1">
@@ -759,13 +762,13 @@
         <v>10</v>
       </c>
       <c r="B23" s="4">
-        <v>85</v>
+        <v>121</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="20" customHeight="1">
@@ -803,13 +806,13 @@
         <v>14</v>
       </c>
       <c r="B27" s="4">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="20" customHeight="1">
@@ -817,10 +820,10 @@
         <v>15</v>
       </c>
       <c r="B28" s="4">
-        <v>92</v>
+        <v>30</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>18</v>
@@ -831,13 +834,13 @@
         <v>16</v>
       </c>
       <c r="B29" s="4">
-        <v>421</v>
+        <v>47</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="20" customHeight="1">
@@ -848,10 +851,10 @@
         <v>30</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="20" customHeight="1">
@@ -879,13 +882,13 @@
         <v>20</v>
       </c>
       <c r="B33" s="4">
-        <v>152</v>
+        <v>85</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="20" customHeight="1">
@@ -893,13 +896,13 @@
         <v>21</v>
       </c>
       <c r="B34" s="4">
-        <v>421</v>
+        <v>121</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="20" customHeight="1">
@@ -910,10 +913,10 @@
         <v>30</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="20" customHeight="1">
@@ -921,13 +924,13 @@
         <v>23</v>
       </c>
       <c r="B36" s="4">
-        <v>92</v>
+        <v>257</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="20" customHeight="1">
@@ -935,10 +938,10 @@
         <v>24</v>
       </c>
       <c r="B37" s="4">
-        <v>121</v>
+        <v>30</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>18</v>
@@ -969,13 +972,13 @@
         <v>27</v>
       </c>
       <c r="B40" s="4">
-        <v>30</v>
+        <v>421</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="20" customHeight="1">
@@ -983,10 +986,10 @@
         <v>28</v>
       </c>
       <c r="B41" s="4">
-        <v>257</v>
+        <v>30</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>18</v>
@@ -997,13 +1000,13 @@
         <v>29</v>
       </c>
       <c r="B42" s="4">
-        <v>356</v>
+        <v>152</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="20" customHeight="1">
@@ -1011,59 +1014,59 @@
         <v>30</v>
       </c>
       <c r="B43" s="4">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="20" customHeight="1">
       <c r="A44" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B44" s="4">
-        <v>3064</v>
+        <v>2549</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="20" customHeight="1">
       <c r="A45" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B45" s="4">
-        <v>241186</v>
+        <v>253557</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="20" customHeight="1">
       <c r="A49" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="20" customHeight="1">
       <c r="A50" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="20" customHeight="1">
       <c r="A51" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="20" customHeight="1">
       <c r="A53" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="20" customHeight="1">
       <c r="A55" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="20" customHeight="1">
       <c r="A57" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
T460 - miercuri 6 iulie 2022, 21:00:03 +0300
</commit_message>
<xml_diff>
--- a/SCRATCH/CLEAN/foaie_parcurs_B-151-VGT_iunie_2022_Alex_Bora.xlsx
+++ b/SCRATCH/CLEAN/foaie_parcurs_B-151-VGT_iunie_2022_Alex_Bora.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="38">
   <si>
     <t>VOLVO ROMÂNIA</t>
   </si>
@@ -76,31 +76,37 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
+    <t>Cluj-Apahida</t>
+  </si>
+  <si>
+    <t>Interes Serviciu</t>
+  </si>
+  <si>
     <t>Cluj-Dej</t>
   </si>
   <si>
-    <t>Interes Serviciu</t>
+    <t>Cluj-Bistrita</t>
+  </si>
+  <si>
+    <t>Cluj-Satu-Mare</t>
+  </si>
+  <si>
+    <t>Cluj-Turda</t>
+  </si>
+  <si>
+    <t>Cluj-Cluj</t>
   </si>
   <si>
     <t>Cluj-Baia-Mare</t>
   </si>
   <si>
+    <t>Cluj-Bontida</t>
+  </si>
+  <si>
+    <t>Cluj-Zalau</t>
+  </si>
+  <si>
     <t>Cluj-Cmp. Turzii</t>
-  </si>
-  <si>
-    <t>Cluj-Turda</t>
-  </si>
-  <si>
-    <t>Cluj-Apahida</t>
-  </si>
-  <si>
-    <t>Cluj-Cluj</t>
-  </si>
-  <si>
-    <t>Cluj-Bistrita</t>
-  </si>
-  <si>
-    <t>Cluj-Satu-Mare</t>
   </si>
   <si>
     <t>Km parcursi:</t>
@@ -626,7 +632,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>251008</v>
+        <v>256004</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="20" customHeight="1">
@@ -672,13 +678,13 @@
         <v>3</v>
       </c>
       <c r="B16" s="4">
-        <v>101</v>
+        <v>30</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="20" customHeight="1">
@@ -706,13 +712,13 @@
         <v>6</v>
       </c>
       <c r="B19" s="4">
-        <v>356</v>
+        <v>30</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="20" customHeight="1">
@@ -720,10 +726,10 @@
         <v>7</v>
       </c>
       <c r="B20" s="4">
-        <v>152</v>
+        <v>85</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>20</v>
@@ -734,13 +740,13 @@
         <v>8</v>
       </c>
       <c r="B21" s="4">
-        <v>30</v>
+        <v>101</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="20" customHeight="1">
@@ -748,10 +754,10 @@
         <v>9</v>
       </c>
       <c r="B22" s="4">
-        <v>356</v>
+        <v>257</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>20</v>
@@ -762,7 +768,7 @@
         <v>10</v>
       </c>
       <c r="B23" s="4">
-        <v>121</v>
+        <v>421</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>23</v>
@@ -806,13 +812,13 @@
         <v>14</v>
       </c>
       <c r="B27" s="4">
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="20" customHeight="1">
@@ -820,13 +826,13 @@
         <v>15</v>
       </c>
       <c r="B28" s="4">
-        <v>30</v>
+        <v>121</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="20" customHeight="1">
@@ -834,10 +840,10 @@
         <v>16</v>
       </c>
       <c r="B29" s="4">
-        <v>47</v>
+        <v>421</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>20</v>
@@ -848,13 +854,13 @@
         <v>17</v>
       </c>
       <c r="B30" s="4">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="20" customHeight="1">
@@ -882,13 +888,13 @@
         <v>20</v>
       </c>
       <c r="B33" s="4">
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="20" customHeight="1">
@@ -896,10 +902,10 @@
         <v>21</v>
       </c>
       <c r="B34" s="4">
-        <v>121</v>
+        <v>356</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>20</v>
@@ -924,13 +930,13 @@
         <v>23</v>
       </c>
       <c r="B36" s="4">
-        <v>257</v>
+        <v>30</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="20" customHeight="1">
@@ -938,13 +944,13 @@
         <v>24</v>
       </c>
       <c r="B37" s="4">
-        <v>30</v>
+        <v>92</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="20" customHeight="1">
@@ -972,10 +978,10 @@
         <v>27</v>
       </c>
       <c r="B40" s="4">
-        <v>421</v>
+        <v>156</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>20</v>
@@ -986,13 +992,13 @@
         <v>28</v>
       </c>
       <c r="B41" s="4">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="20" customHeight="1">
@@ -1000,13 +1006,13 @@
         <v>29</v>
       </c>
       <c r="B42" s="4">
-        <v>152</v>
+        <v>30</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="20" customHeight="1">
@@ -1014,10 +1020,10 @@
         <v>30</v>
       </c>
       <c r="B43" s="4">
-        <v>85</v>
+        <v>152</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>20</v>
@@ -1025,48 +1031,48 @@
     </row>
     <row r="44" spans="1:4" ht="20" customHeight="1">
       <c r="A44" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B44" s="4">
-        <v>2549</v>
+        <v>2534</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="20" customHeight="1">
       <c r="A45" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B45" s="4">
-        <v>253557</v>
+        <v>258538</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="20" customHeight="1">
       <c r="A49" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="20" customHeight="1">
       <c r="A50" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="20" customHeight="1">
       <c r="A51" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="20" customHeight="1">
       <c r="A53" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="20" customHeight="1">
       <c r="A55" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="20" customHeight="1">
       <c r="A57" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
T460 - joi 7 iulie 2022, 09:44:55 +0300
</commit_message>
<xml_diff>
--- a/SCRATCH/CLEAN/foaie_parcurs_B-151-VGT_iunie_2022_Alex_Bora.xlsx
+++ b/SCRATCH/CLEAN/foaie_parcurs_B-151-VGT_iunie_2022_Alex_Bora.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="35">
   <si>
     <t>VOLVO ROMÂNIA</t>
   </si>
@@ -70,43 +70,34 @@
     <t>Observatii utilizator</t>
   </si>
   <si>
+    <t>Cluj-Zalau</t>
+  </si>
+  <si>
+    <t>Interes Serviciu</t>
+  </si>
+  <si>
+    <t>Cluj-Cmp. Turzii</t>
+  </si>
+  <si>
+    <t>Cluj-Satu-Mare</t>
+  </si>
+  <si>
+    <t>Cluj-Baia-Mare</t>
+  </si>
+  <si>
+    <t>Cluj-Turda</t>
+  </si>
+  <si>
     <t>Acasa-Birou</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Cluj-Apahida</t>
-  </si>
-  <si>
-    <t>Interes Serviciu</t>
-  </si>
-  <si>
-    <t>Cluj-Dej</t>
-  </si>
-  <si>
     <t>Cluj-Bistrita</t>
   </si>
   <si>
-    <t>Cluj-Satu-Mare</t>
-  </si>
-  <si>
-    <t>Cluj-Turda</t>
-  </si>
-  <si>
     <t>Cluj-Cluj</t>
-  </si>
-  <si>
-    <t>Cluj-Baia-Mare</t>
-  </si>
-  <si>
-    <t>Cluj-Bontida</t>
-  </si>
-  <si>
-    <t>Cluj-Zalau</t>
-  </si>
-  <si>
-    <t>Cluj-Cmp. Turzii</t>
   </si>
   <si>
     <t>Km parcursi:</t>
@@ -632,7 +623,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>256004</v>
+        <v>263351</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="20" customHeight="1">
@@ -664,7 +655,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="4">
-        <v>30</v>
+        <v>156</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>17</v>
@@ -678,10 +669,10 @@
         <v>3</v>
       </c>
       <c r="B16" s="4">
-        <v>30</v>
+        <v>152</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>18</v>
@@ -712,10 +703,10 @@
         <v>6</v>
       </c>
       <c r="B19" s="4">
-        <v>30</v>
+        <v>421</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>18</v>
@@ -726,13 +717,13 @@
         <v>7</v>
       </c>
       <c r="B20" s="4">
-        <v>85</v>
+        <v>356</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="20" customHeight="1">
@@ -740,13 +731,13 @@
         <v>8</v>
       </c>
       <c r="B21" s="4">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="20" customHeight="1">
@@ -754,13 +745,13 @@
         <v>9</v>
       </c>
       <c r="B22" s="4">
-        <v>257</v>
+        <v>156</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="20" customHeight="1">
@@ -768,13 +759,13 @@
         <v>10</v>
       </c>
       <c r="B23" s="4">
-        <v>421</v>
+        <v>356</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="20" customHeight="1">
@@ -812,10 +803,10 @@
         <v>14</v>
       </c>
       <c r="B27" s="4">
-        <v>30</v>
+        <v>121</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>18</v>
@@ -826,13 +817,13 @@
         <v>15</v>
       </c>
       <c r="B28" s="4">
-        <v>121</v>
+        <v>30</v>
       </c>
       <c r="C28" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="20" customHeight="1">
@@ -840,13 +831,13 @@
         <v>16</v>
       </c>
       <c r="B29" s="4">
-        <v>421</v>
+        <v>152</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="20" customHeight="1">
@@ -854,13 +845,13 @@
         <v>17</v>
       </c>
       <c r="B30" s="4">
-        <v>47</v>
+        <v>257</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="20" customHeight="1">
@@ -888,10 +879,10 @@
         <v>20</v>
       </c>
       <c r="B33" s="4">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>18</v>
@@ -902,13 +893,13 @@
         <v>21</v>
       </c>
       <c r="B34" s="4">
-        <v>356</v>
+        <v>421</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="20" customHeight="1">
@@ -919,10 +910,10 @@
         <v>30</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="20" customHeight="1">
@@ -930,10 +921,10 @@
         <v>23</v>
       </c>
       <c r="B36" s="4">
-        <v>30</v>
+        <v>421</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>18</v>
@@ -944,13 +935,13 @@
         <v>24</v>
       </c>
       <c r="B37" s="4">
-        <v>92</v>
+        <v>30</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="20" customHeight="1">
@@ -978,13 +969,13 @@
         <v>27</v>
       </c>
       <c r="B40" s="4">
-        <v>156</v>
+        <v>30</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="20" customHeight="1">
@@ -992,13 +983,13 @@
         <v>28</v>
       </c>
       <c r="B41" s="4">
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="20" customHeight="1">
@@ -1006,10 +997,10 @@
         <v>29</v>
       </c>
       <c r="B42" s="4">
-        <v>30</v>
+        <v>421</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>18</v>
@@ -1020,59 +1011,59 @@
         <v>30</v>
       </c>
       <c r="B43" s="4">
-        <v>152</v>
+        <v>257</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="20" customHeight="1">
       <c r="A44" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B44" s="4">
-        <v>2534</v>
+        <v>3965</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="20" customHeight="1">
       <c r="A45" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B45" s="4">
-        <v>258538</v>
+        <v>267316</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="20" customHeight="1">
       <c r="A49" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="20" customHeight="1">
       <c r="A50" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="20" customHeight="1">
       <c r="A51" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="20" customHeight="1">
       <c r="A53" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="20" customHeight="1">
       <c r="A55" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="20" customHeight="1">
       <c r="A57" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
T460 - joi 7 iulie 2022, 09:52:52 +0300
</commit_message>
<xml_diff>
--- a/SCRATCH/CLEAN/foaie_parcurs_B-151-VGT_iunie_2022_Alex_Bora.xlsx
+++ b/SCRATCH/CLEAN/foaie_parcurs_B-151-VGT_iunie_2022_Alex_Bora.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="37">
   <si>
     <t>VOLVO ROMÂNIA</t>
   </si>
@@ -76,28 +76,34 @@
     <t>Interes Serviciu</t>
   </si>
   <si>
+    <t>Cluj-Cluj</t>
+  </si>
+  <si>
+    <t>Acasa-Birou</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Cluj-Turda</t>
+  </si>
+  <si>
+    <t>Cluj-Dej</t>
+  </si>
+  <si>
+    <t>Cluj-Bontida</t>
+  </si>
+  <si>
+    <t>Cluj-Bistrita</t>
+  </si>
+  <si>
+    <t>Cluj-Apahida</t>
+  </si>
+  <si>
     <t>Cluj-Cmp. Turzii</t>
   </si>
   <si>
     <t>Cluj-Satu-Mare</t>
-  </si>
-  <si>
-    <t>Cluj-Baia-Mare</t>
-  </si>
-  <si>
-    <t>Cluj-Turda</t>
-  </si>
-  <si>
-    <t>Acasa-Birou</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Cluj-Bistrita</t>
-  </si>
-  <si>
-    <t>Cluj-Cluj</t>
   </si>
   <si>
     <t>Km parcursi:</t>
@@ -623,7 +629,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>263351</v>
+        <v>267316</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="20" customHeight="1">
@@ -669,7 +675,7 @@
         <v>3</v>
       </c>
       <c r="B16" s="4">
-        <v>152</v>
+        <v>47</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>19</v>
@@ -703,13 +709,13 @@
         <v>6</v>
       </c>
       <c r="B19" s="4">
-        <v>421</v>
+        <v>30</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="20" customHeight="1">
@@ -717,10 +723,10 @@
         <v>7</v>
       </c>
       <c r="B20" s="4">
-        <v>356</v>
+        <v>121</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>18</v>
@@ -731,10 +737,10 @@
         <v>8</v>
       </c>
       <c r="B21" s="4">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>18</v>
@@ -759,10 +765,10 @@
         <v>10</v>
       </c>
       <c r="B23" s="4">
-        <v>356</v>
+        <v>92</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>18</v>
@@ -803,10 +809,10 @@
         <v>14</v>
       </c>
       <c r="B27" s="4">
-        <v>121</v>
+        <v>257</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>18</v>
@@ -817,13 +823,13 @@
         <v>15</v>
       </c>
       <c r="B28" s="4">
-        <v>30</v>
+        <v>101</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="20" customHeight="1">
@@ -831,10 +837,10 @@
         <v>16</v>
       </c>
       <c r="B29" s="4">
-        <v>152</v>
+        <v>85</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>18</v>
@@ -845,13 +851,13 @@
         <v>17</v>
       </c>
       <c r="B30" s="4">
-        <v>257</v>
+        <v>30</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="20" customHeight="1">
@@ -879,13 +885,13 @@
         <v>20</v>
       </c>
       <c r="B33" s="4">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="20" customHeight="1">
@@ -893,10 +899,10 @@
         <v>21</v>
       </c>
       <c r="B34" s="4">
-        <v>421</v>
+        <v>152</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>18</v>
@@ -907,13 +913,13 @@
         <v>22</v>
       </c>
       <c r="B35" s="4">
-        <v>30</v>
+        <v>257</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="20" customHeight="1">
@@ -921,13 +927,13 @@
         <v>23</v>
       </c>
       <c r="B36" s="4">
-        <v>421</v>
+        <v>30</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="20" customHeight="1">
@@ -935,13 +941,13 @@
         <v>24</v>
       </c>
       <c r="B37" s="4">
-        <v>30</v>
+        <v>257</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="20" customHeight="1">
@@ -969,13 +975,13 @@
         <v>27</v>
       </c>
       <c r="B40" s="4">
-        <v>30</v>
+        <v>421</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="20" customHeight="1">
@@ -986,10 +992,10 @@
         <v>30</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="20" customHeight="1">
@@ -997,13 +1003,13 @@
         <v>29</v>
       </c>
       <c r="B42" s="4">
-        <v>421</v>
+        <v>30</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="20" customHeight="1">
@@ -1011,10 +1017,10 @@
         <v>30</v>
       </c>
       <c r="B43" s="4">
-        <v>257</v>
+        <v>121</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>18</v>
@@ -1022,48 +1028,48 @@
     </row>
     <row r="44" spans="1:4" ht="20" customHeight="1">
       <c r="A44" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B44" s="4">
-        <v>3965</v>
+        <v>2504</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="20" customHeight="1">
       <c r="A45" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B45" s="4">
-        <v>267316</v>
+        <v>269820</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="20" customHeight="1">
       <c r="A49" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="20" customHeight="1">
       <c r="A50" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="20" customHeight="1">
       <c r="A51" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="20" customHeight="1">
       <c r="A53" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="20" customHeight="1">
       <c r="A55" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="20" customHeight="1">
       <c r="A57" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
T460 - vineri 8 iulie 2022, 20:18:00 +0300
</commit_message>
<xml_diff>
--- a/SCRATCH/CLEAN/foaie_parcurs_B-151-VGT_iunie_2022_Alex_Bora.xlsx
+++ b/SCRATCH/CLEAN/foaie_parcurs_B-151-VGT_iunie_2022_Alex_Bora.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="34">
   <si>
     <t>VOLVO ROMÂNIA</t>
   </si>
@@ -70,40 +70,31 @@
     <t>Observatii utilizator</t>
   </si>
   <si>
-    <t>Cluj-Zalau</t>
+    <t>Cluj-Bistrita</t>
   </si>
   <si>
     <t>Interes Serviciu</t>
   </si>
   <si>
+    <t>Acasa-Birou</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Cluj-Turda</t>
+  </si>
+  <si>
+    <t>Cluj-Satu-Mare</t>
+  </si>
+  <si>
+    <t>Cluj-Cmp. Turzii</t>
+  </si>
+  <si>
+    <t>Cluj-Baia-Mare</t>
+  </si>
+  <si>
     <t>Cluj-Cluj</t>
-  </si>
-  <si>
-    <t>Acasa-Birou</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Cluj-Turda</t>
-  </si>
-  <si>
-    <t>Cluj-Dej</t>
-  </si>
-  <si>
-    <t>Cluj-Bontida</t>
-  </si>
-  <si>
-    <t>Cluj-Bistrita</t>
-  </si>
-  <si>
-    <t>Cluj-Apahida</t>
-  </si>
-  <si>
-    <t>Cluj-Cmp. Turzii</t>
-  </si>
-  <si>
-    <t>Cluj-Satu-Mare</t>
   </si>
   <si>
     <t>Km parcursi:</t>
@@ -629,7 +620,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>267316</v>
+        <v>283618</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="20" customHeight="1">
@@ -661,7 +652,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="4">
-        <v>156</v>
+        <v>257</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>17</v>
@@ -675,13 +666,13 @@
         <v>3</v>
       </c>
       <c r="B16" s="4">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="20" customHeight="1">
@@ -712,10 +703,10 @@
         <v>30</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="20" customHeight="1">
@@ -723,10 +714,10 @@
         <v>7</v>
       </c>
       <c r="B20" s="4">
-        <v>121</v>
+        <v>257</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>18</v>
@@ -737,10 +728,10 @@
         <v>8</v>
       </c>
       <c r="B21" s="4">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>18</v>
@@ -751,13 +742,13 @@
         <v>9</v>
       </c>
       <c r="B22" s="4">
-        <v>156</v>
+        <v>30</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="20" customHeight="1">
@@ -765,13 +756,13 @@
         <v>10</v>
       </c>
       <c r="B23" s="4">
-        <v>92</v>
+        <v>30</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="20" customHeight="1">
@@ -809,13 +800,13 @@
         <v>14</v>
       </c>
       <c r="B27" s="4">
-        <v>257</v>
+        <v>30</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="20" customHeight="1">
@@ -823,10 +814,10 @@
         <v>15</v>
       </c>
       <c r="B28" s="4">
-        <v>101</v>
+        <v>421</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>18</v>
@@ -837,13 +828,13 @@
         <v>16</v>
       </c>
       <c r="B29" s="4">
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="20" customHeight="1">
@@ -851,13 +842,13 @@
         <v>17</v>
       </c>
       <c r="B30" s="4">
-        <v>30</v>
+        <v>152</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="20" customHeight="1">
@@ -885,13 +876,13 @@
         <v>20</v>
       </c>
       <c r="B33" s="4">
-        <v>30</v>
+        <v>421</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="20" customHeight="1">
@@ -899,13 +890,13 @@
         <v>21</v>
       </c>
       <c r="B34" s="4">
-        <v>152</v>
+        <v>30</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="20" customHeight="1">
@@ -913,13 +904,13 @@
         <v>22</v>
       </c>
       <c r="B35" s="4">
-        <v>257</v>
+        <v>30</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="20" customHeight="1">
@@ -930,10 +921,10 @@
         <v>30</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="20" customHeight="1">
@@ -941,10 +932,10 @@
         <v>24</v>
       </c>
       <c r="B37" s="4">
-        <v>257</v>
+        <v>356</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>18</v>
@@ -975,10 +966,10 @@
         <v>27</v>
       </c>
       <c r="B40" s="4">
-        <v>421</v>
+        <v>47</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>18</v>
@@ -992,10 +983,10 @@
         <v>30</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="20" customHeight="1">
@@ -1006,10 +997,10 @@
         <v>30</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="20" customHeight="1">
@@ -1017,59 +1008,59 @@
         <v>30</v>
       </c>
       <c r="B43" s="4">
-        <v>121</v>
+        <v>30</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="20" customHeight="1">
       <c r="A44" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B44" s="4">
-        <v>2504</v>
+        <v>2392</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="20" customHeight="1">
       <c r="A45" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B45" s="4">
-        <v>269820</v>
+        <v>286010</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="20" customHeight="1">
       <c r="A49" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="20" customHeight="1">
       <c r="A50" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="20" customHeight="1">
       <c r="A51" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="20" customHeight="1">
       <c r="A53" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="20" customHeight="1">
       <c r="A55" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="20" customHeight="1">
       <c r="A57" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
T460 - vineri 8 iulie 2022, 20:28:16 +0300
</commit_message>
<xml_diff>
--- a/SCRATCH/CLEAN/foaie_parcurs_B-151-VGT_iunie_2022_Alex_Bora.xlsx
+++ b/SCRATCH/CLEAN/foaie_parcurs_B-151-VGT_iunie_2022_Alex_Bora.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
   <si>
     <t>VOLVO ROMÂNIA</t>
   </si>
@@ -70,31 +70,37 @@
     <t>Observatii utilizator</t>
   </si>
   <si>
+    <t>Cluj-Cmp. Turzii</t>
+  </si>
+  <si>
+    <t>Interes Serviciu</t>
+  </si>
+  <si>
+    <t>Cluj-Cluj</t>
+  </si>
+  <si>
+    <t>Cluj-Turda</t>
+  </si>
+  <si>
+    <t>Acasa-Birou</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Cluj-Bontida</t>
+  </si>
+  <si>
+    <t>Cluj-Baia-Mare</t>
+  </si>
+  <si>
     <t>Cluj-Bistrita</t>
   </si>
   <si>
-    <t>Interes Serviciu</t>
-  </si>
-  <si>
-    <t>Acasa-Birou</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Cluj-Turda</t>
-  </si>
-  <si>
-    <t>Cluj-Satu-Mare</t>
-  </si>
-  <si>
-    <t>Cluj-Cmp. Turzii</t>
-  </si>
-  <si>
-    <t>Cluj-Baia-Mare</t>
-  </si>
-  <si>
-    <t>Cluj-Cluj</t>
+    <t>Cluj-Apahida</t>
+  </si>
+  <si>
+    <t>Cluj-Zalau</t>
   </si>
   <si>
     <t>Km parcursi:</t>
@@ -620,7 +626,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>283618</v>
+        <v>286010</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="20" customHeight="1">
@@ -652,7 +658,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="4">
-        <v>257</v>
+        <v>152</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>17</v>
@@ -666,13 +672,13 @@
         <v>3</v>
       </c>
       <c r="B16" s="4">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="20" customHeight="1">
@@ -700,13 +706,13 @@
         <v>6</v>
       </c>
       <c r="B19" s="4">
-        <v>30</v>
+        <v>121</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="20" customHeight="1">
@@ -714,13 +720,13 @@
         <v>7</v>
       </c>
       <c r="B20" s="4">
-        <v>257</v>
+        <v>30</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="20" customHeight="1">
@@ -728,10 +734,10 @@
         <v>8</v>
       </c>
       <c r="B21" s="4">
-        <v>121</v>
+        <v>92</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>18</v>
@@ -742,13 +748,13 @@
         <v>9</v>
       </c>
       <c r="B22" s="4">
-        <v>30</v>
+        <v>121</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="20" customHeight="1">
@@ -759,10 +765,10 @@
         <v>30</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="20" customHeight="1">
@@ -800,13 +806,13 @@
         <v>14</v>
       </c>
       <c r="B27" s="4">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="20" customHeight="1">
@@ -814,13 +820,13 @@
         <v>15</v>
       </c>
       <c r="B28" s="4">
-        <v>421</v>
+        <v>30</v>
       </c>
       <c r="C28" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="20" customHeight="1">
@@ -828,13 +834,13 @@
         <v>16</v>
       </c>
       <c r="B29" s="4">
-        <v>30</v>
+        <v>356</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="20" customHeight="1">
@@ -842,13 +848,13 @@
         <v>17</v>
       </c>
       <c r="B30" s="4">
-        <v>152</v>
+        <v>30</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="20" customHeight="1">
@@ -876,10 +882,10 @@
         <v>20</v>
       </c>
       <c r="B33" s="4">
-        <v>421</v>
+        <v>121</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>18</v>
@@ -890,13 +896,13 @@
         <v>21</v>
       </c>
       <c r="B34" s="4">
-        <v>30</v>
+        <v>257</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="20" customHeight="1">
@@ -904,13 +910,13 @@
         <v>22</v>
       </c>
       <c r="B35" s="4">
-        <v>30</v>
+        <v>152</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="20" customHeight="1">
@@ -918,13 +924,13 @@
         <v>23</v>
       </c>
       <c r="B36" s="4">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="20" customHeight="1">
@@ -932,10 +938,10 @@
         <v>24</v>
       </c>
       <c r="B37" s="4">
-        <v>356</v>
+        <v>92</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>18</v>
@@ -966,10 +972,10 @@
         <v>27</v>
       </c>
       <c r="B40" s="4">
-        <v>47</v>
+        <v>121</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>18</v>
@@ -980,13 +986,13 @@
         <v>28</v>
       </c>
       <c r="B41" s="4">
-        <v>30</v>
+        <v>156</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="20" customHeight="1">
@@ -994,13 +1000,13 @@
         <v>29</v>
       </c>
       <c r="B42" s="4">
-        <v>30</v>
+        <v>152</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="20" customHeight="1">
@@ -1011,56 +1017,56 @@
         <v>30</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="20" customHeight="1">
       <c r="A44" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B44" s="4">
-        <v>2392</v>
+        <v>2222</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="20" customHeight="1">
       <c r="A45" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B45" s="4">
-        <v>286010</v>
+        <v>288232</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="20" customHeight="1">
       <c r="A49" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="20" customHeight="1">
       <c r="A50" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="20" customHeight="1">
       <c r="A51" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="20" customHeight="1">
       <c r="A53" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="20" customHeight="1">
       <c r="A55" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="20" customHeight="1">
       <c r="A57" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
T460 - vineri 8 iulie 2022, 21:03:09 +0300
</commit_message>
<xml_diff>
--- a/SCRATCH/CLEAN/foaie_parcurs_B-151-VGT_iunie_2022_Alex_Bora.xlsx
+++ b/SCRATCH/CLEAN/foaie_parcurs_B-151-VGT_iunie_2022_Alex_Bora.xlsx
@@ -70,37 +70,37 @@
     <t>Observatii utilizator</t>
   </si>
   <si>
+    <t>Acasa-Birou</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Cluj-Turda</t>
+  </si>
+  <si>
+    <t>Interes Serviciu</t>
+  </si>
+  <si>
+    <t>Cluj-Baia-Mare</t>
+  </si>
+  <si>
+    <t>Cluj-Cluj</t>
+  </si>
+  <si>
+    <t>Cluj-Zalau</t>
+  </si>
+  <si>
+    <t>Cluj-Apahida</t>
+  </si>
+  <si>
+    <t>Cluj-Bistrita</t>
+  </si>
+  <si>
     <t>Cluj-Cmp. Turzii</t>
   </si>
   <si>
-    <t>Interes Serviciu</t>
-  </si>
-  <si>
-    <t>Cluj-Cluj</t>
-  </si>
-  <si>
-    <t>Cluj-Turda</t>
-  </si>
-  <si>
-    <t>Acasa-Birou</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Cluj-Bontida</t>
-  </si>
-  <si>
-    <t>Cluj-Baia-Mare</t>
-  </si>
-  <si>
-    <t>Cluj-Bistrita</t>
-  </si>
-  <si>
-    <t>Cluj-Apahida</t>
-  </si>
-  <si>
-    <t>Cluj-Zalau</t>
+    <t>Cluj-Satu-Mare</t>
   </si>
   <si>
     <t>Km parcursi:</t>
@@ -626,7 +626,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>286010</v>
+        <v>290326</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="20" customHeight="1">
@@ -658,7 +658,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="4">
-        <v>152</v>
+        <v>30</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>17</v>
@@ -672,13 +672,13 @@
         <v>3</v>
       </c>
       <c r="B16" s="4">
-        <v>47</v>
+        <v>121</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="20" customHeight="1">
@@ -709,10 +709,10 @@
         <v>121</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="20" customHeight="1">
@@ -720,13 +720,13 @@
         <v>7</v>
       </c>
       <c r="B20" s="4">
-        <v>30</v>
+        <v>356</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="20" customHeight="1">
@@ -734,10 +734,10 @@
         <v>8</v>
       </c>
       <c r="B21" s="4">
-        <v>92</v>
+        <v>30</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>18</v>
@@ -748,13 +748,13 @@
         <v>9</v>
       </c>
       <c r="B22" s="4">
-        <v>121</v>
+        <v>47</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="20" customHeight="1">
@@ -762,13 +762,13 @@
         <v>10</v>
       </c>
       <c r="B23" s="4">
-        <v>30</v>
+        <v>156</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="20" customHeight="1">
@@ -806,10 +806,10 @@
         <v>14</v>
       </c>
       <c r="B27" s="4">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>18</v>
@@ -820,13 +820,13 @@
         <v>15</v>
       </c>
       <c r="B28" s="4">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="20" customHeight="1">
@@ -834,13 +834,13 @@
         <v>16</v>
       </c>
       <c r="B29" s="4">
-        <v>356</v>
+        <v>257</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="20" customHeight="1">
@@ -848,13 +848,13 @@
         <v>17</v>
       </c>
       <c r="B30" s="4">
-        <v>30</v>
+        <v>356</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="20" customHeight="1">
@@ -882,13 +882,13 @@
         <v>20</v>
       </c>
       <c r="B33" s="4">
-        <v>121</v>
+        <v>152</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="20" customHeight="1">
@@ -896,13 +896,13 @@
         <v>21</v>
       </c>
       <c r="B34" s="4">
-        <v>257</v>
+        <v>421</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="20" customHeight="1">
@@ -910,13 +910,13 @@
         <v>22</v>
       </c>
       <c r="B35" s="4">
-        <v>152</v>
+        <v>257</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="20" customHeight="1">
@@ -924,10 +924,10 @@
         <v>23</v>
       </c>
       <c r="B36" s="4">
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>18</v>
@@ -938,13 +938,13 @@
         <v>24</v>
       </c>
       <c r="B37" s="4">
-        <v>92</v>
+        <v>121</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="20" customHeight="1">
@@ -972,10 +972,10 @@
         <v>27</v>
       </c>
       <c r="B40" s="4">
-        <v>121</v>
+        <v>30</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>18</v>
@@ -986,10 +986,10 @@
         <v>28</v>
       </c>
       <c r="B41" s="4">
-        <v>156</v>
+        <v>30</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>18</v>
@@ -1000,13 +1000,13 @@
         <v>29</v>
       </c>
       <c r="B42" s="4">
-        <v>152</v>
+        <v>421</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="20" customHeight="1">
@@ -1017,10 +1017,10 @@
         <v>30</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="20" customHeight="1">
@@ -1028,7 +1028,7 @@
         <v>28</v>
       </c>
       <c r="B44" s="4">
-        <v>2222</v>
+        <v>3081</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="20" customHeight="1">
@@ -1036,7 +1036,7 @@
         <v>29</v>
       </c>
       <c r="B45" s="4">
-        <v>288232</v>
+        <v>293407</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="20" customHeight="1">

</xml_diff>

<commit_message>
T460 -  sâmbătă 9 iulie 2022, 09:27:23 +0300
</commit_message>
<xml_diff>
--- a/SCRATCH/CLEAN/foaie_parcurs_B-151-VGT_iunie_2022_Alex_Bora.xlsx
+++ b/SCRATCH/CLEAN/foaie_parcurs_B-151-VGT_iunie_2022_Alex_Bora.xlsx
@@ -70,37 +70,37 @@
     <t>Observatii utilizator</t>
   </si>
   <si>
+    <t>Cluj-Bontida</t>
+  </si>
+  <si>
+    <t>Interes Serviciu</t>
+  </si>
+  <si>
+    <t>Cluj-Cmp. Turzii</t>
+  </si>
+  <si>
+    <t>Cluj-Apahida</t>
+  </si>
+  <si>
     <t>Acasa-Birou</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Cluj-Turda</t>
-  </si>
-  <si>
-    <t>Interes Serviciu</t>
+    <t>Cluj-Satu-Mare</t>
+  </si>
+  <si>
+    <t>Cluj-Zalau</t>
+  </si>
+  <si>
+    <t>Cluj-Dej</t>
   </si>
   <si>
     <t>Cluj-Baia-Mare</t>
   </si>
   <si>
-    <t>Cluj-Cluj</t>
-  </si>
-  <si>
-    <t>Cluj-Zalau</t>
-  </si>
-  <si>
-    <t>Cluj-Apahida</t>
-  </si>
-  <si>
     <t>Cluj-Bistrita</t>
-  </si>
-  <si>
-    <t>Cluj-Cmp. Turzii</t>
-  </si>
-  <si>
-    <t>Cluj-Satu-Mare</t>
   </si>
   <si>
     <t>Km parcursi:</t>
@@ -626,7 +626,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>290326</v>
+        <v>300632</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="20" customHeight="1">
@@ -658,7 +658,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="4">
-        <v>30</v>
+        <v>92</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>17</v>
@@ -672,13 +672,13 @@
         <v>3</v>
       </c>
       <c r="B16" s="4">
-        <v>121</v>
+        <v>152</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="20" customHeight="1">
@@ -706,13 +706,13 @@
         <v>6</v>
       </c>
       <c r="B19" s="4">
-        <v>121</v>
+        <v>85</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="20" customHeight="1">
@@ -720,13 +720,13 @@
         <v>7</v>
       </c>
       <c r="B20" s="4">
-        <v>356</v>
+        <v>30</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="20" customHeight="1">
@@ -734,10 +734,10 @@
         <v>8</v>
       </c>
       <c r="B21" s="4">
-        <v>30</v>
+        <v>421</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>18</v>
@@ -748,13 +748,13 @@
         <v>9</v>
       </c>
       <c r="B22" s="4">
-        <v>47</v>
+        <v>156</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="20" customHeight="1">
@@ -762,13 +762,13 @@
         <v>10</v>
       </c>
       <c r="B23" s="4">
-        <v>156</v>
+        <v>101</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="20" customHeight="1">
@@ -809,10 +809,10 @@
         <v>30</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="20" customHeight="1">
@@ -820,13 +820,13 @@
         <v>15</v>
       </c>
       <c r="B28" s="4">
-        <v>85</v>
+        <v>356</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="20" customHeight="1">
@@ -834,13 +834,13 @@
         <v>16</v>
       </c>
       <c r="B29" s="4">
-        <v>257</v>
+        <v>152</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="20" customHeight="1">
@@ -848,13 +848,13 @@
         <v>17</v>
       </c>
       <c r="B30" s="4">
-        <v>356</v>
+        <v>30</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="20" customHeight="1">
@@ -882,13 +882,13 @@
         <v>20</v>
       </c>
       <c r="B33" s="4">
-        <v>152</v>
+        <v>356</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="20" customHeight="1">
@@ -896,13 +896,13 @@
         <v>21</v>
       </c>
       <c r="B34" s="4">
-        <v>421</v>
+        <v>152</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="20" customHeight="1">
@@ -910,13 +910,13 @@
         <v>22</v>
       </c>
       <c r="B35" s="4">
-        <v>257</v>
+        <v>356</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="20" customHeight="1">
@@ -924,10 +924,10 @@
         <v>23</v>
       </c>
       <c r="B36" s="4">
-        <v>30</v>
+        <v>257</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>18</v>
@@ -938,13 +938,13 @@
         <v>24</v>
       </c>
       <c r="B37" s="4">
-        <v>121</v>
+        <v>30</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="20" customHeight="1">
@@ -972,10 +972,10 @@
         <v>27</v>
       </c>
       <c r="B40" s="4">
-        <v>30</v>
+        <v>356</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>18</v>
@@ -989,10 +989,10 @@
         <v>30</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="20" customHeight="1">
@@ -1000,13 +1000,13 @@
         <v>29</v>
       </c>
       <c r="B42" s="4">
-        <v>421</v>
+        <v>30</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="20" customHeight="1">
@@ -1014,10 +1014,10 @@
         <v>30</v>
       </c>
       <c r="B43" s="4">
-        <v>30</v>
+        <v>356</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>18</v>
@@ -1028,7 +1028,7 @@
         <v>28</v>
       </c>
       <c r="B44" s="4">
-        <v>3081</v>
+        <v>3528</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="20" customHeight="1">
@@ -1036,7 +1036,7 @@
         <v>29</v>
       </c>
       <c r="B45" s="4">
-        <v>293407</v>
+        <v>304160</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="20" customHeight="1">

</xml_diff>

<commit_message>
T460 - sâmbătă 9 iulie 2022, 12:10:58 +0300
</commit_message>
<xml_diff>
--- a/SCRATCH/CLEAN/foaie_parcurs_B-151-VGT_iunie_2022_Alex_Bora.xlsx
+++ b/SCRATCH/CLEAN/foaie_parcurs_B-151-VGT_iunie_2022_Alex_Bora.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="37">
   <si>
     <t>VOLVO ROMÂNIA</t>
   </si>
@@ -70,37 +70,40 @@
     <t>Observatii utilizator</t>
   </si>
   <si>
+    <t>Cluj-Apahida</t>
+  </si>
+  <si>
+    <t>Interes Serviciu</t>
+  </si>
+  <si>
+    <t>Cluj-Cluj</t>
+  </si>
+  <si>
     <t>Cluj-Bontida</t>
   </si>
   <si>
-    <t>Interes Serviciu</t>
+    <t>Cluj-Bistrita</t>
+  </si>
+  <si>
+    <t>Acasa-Birou</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Cluj-Satu-Mare</t>
   </si>
   <si>
     <t>Cluj-Cmp. Turzii</t>
   </si>
   <si>
-    <t>Cluj-Apahida</t>
-  </si>
-  <si>
-    <t>Acasa-Birou</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Cluj-Satu-Mare</t>
+    <t>Cluj-Turda</t>
+  </si>
+  <si>
+    <t>Cluj-Baia-Mare</t>
   </si>
   <si>
     <t>Cluj-Zalau</t>
-  </si>
-  <si>
-    <t>Cluj-Dej</t>
-  </si>
-  <si>
-    <t>Cluj-Baia-Mare</t>
-  </si>
-  <si>
-    <t>Cluj-Bistrita</t>
   </si>
   <si>
     <t>Km parcursi:</t>
@@ -626,7 +629,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>300632</v>
+        <v>307760</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="20" customHeight="1">
@@ -658,7 +661,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="4">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>17</v>
@@ -672,7 +675,7 @@
         <v>3</v>
       </c>
       <c r="B16" s="4">
-        <v>152</v>
+        <v>47</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>19</v>
@@ -706,7 +709,7 @@
         <v>6</v>
       </c>
       <c r="B19" s="4">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>20</v>
@@ -720,13 +723,13 @@
         <v>7</v>
       </c>
       <c r="B20" s="4">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="20" customHeight="1">
@@ -734,10 +737,10 @@
         <v>8</v>
       </c>
       <c r="B21" s="4">
-        <v>421</v>
+        <v>257</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>18</v>
@@ -748,13 +751,13 @@
         <v>9</v>
       </c>
       <c r="B22" s="4">
-        <v>156</v>
+        <v>30</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="20" customHeight="1">
@@ -762,13 +765,13 @@
         <v>10</v>
       </c>
       <c r="B23" s="4">
-        <v>101</v>
+        <v>30</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="20" customHeight="1">
@@ -806,13 +809,13 @@
         <v>14</v>
       </c>
       <c r="B27" s="4">
-        <v>30</v>
+        <v>421</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="20" customHeight="1">
@@ -820,10 +823,10 @@
         <v>15</v>
       </c>
       <c r="B28" s="4">
-        <v>356</v>
+        <v>152</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>18</v>
@@ -834,13 +837,13 @@
         <v>16</v>
       </c>
       <c r="B29" s="4">
-        <v>152</v>
+        <v>30</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="20" customHeight="1">
@@ -848,13 +851,13 @@
         <v>17</v>
       </c>
       <c r="B30" s="4">
-        <v>30</v>
+        <v>121</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="20" customHeight="1">
@@ -882,13 +885,13 @@
         <v>20</v>
       </c>
       <c r="B33" s="4">
-        <v>356</v>
+        <v>30</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="20" customHeight="1">
@@ -896,10 +899,10 @@
         <v>21</v>
       </c>
       <c r="B34" s="4">
-        <v>152</v>
+        <v>92</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>18</v>
@@ -913,7 +916,7 @@
         <v>356</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>18</v>
@@ -924,10 +927,10 @@
         <v>23</v>
       </c>
       <c r="B36" s="4">
-        <v>257</v>
+        <v>156</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>18</v>
@@ -938,13 +941,13 @@
         <v>24</v>
       </c>
       <c r="B37" s="4">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="20" customHeight="1">
@@ -972,7 +975,7 @@
         <v>27</v>
       </c>
       <c r="B40" s="4">
-        <v>356</v>
+        <v>121</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>26</v>
@@ -986,13 +989,13 @@
         <v>28</v>
       </c>
       <c r="B41" s="4">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="20" customHeight="1">
@@ -1003,10 +1006,10 @@
         <v>30</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="20" customHeight="1">
@@ -1014,59 +1017,59 @@
         <v>30</v>
       </c>
       <c r="B43" s="4">
-        <v>356</v>
+        <v>30</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="20" customHeight="1">
       <c r="A44" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B44" s="4">
-        <v>3528</v>
+        <v>2259</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="20" customHeight="1">
       <c r="A45" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B45" s="4">
-        <v>304160</v>
+        <v>310019</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="20" customHeight="1">
       <c r="A49" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="20" customHeight="1">
       <c r="A50" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="20" customHeight="1">
       <c r="A51" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="20" customHeight="1">
       <c r="A53" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="20" customHeight="1">
       <c r="A55" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="20" customHeight="1">
       <c r="A57" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
T460 -  duminică 10 iulie 2022, 14:17:17 +0300
</commit_message>
<xml_diff>
--- a/SCRATCH/CLEAN/foaie_parcurs_B-151-VGT_iunie_2022_Alex_Bora.xlsx
+++ b/SCRATCH/CLEAN/foaie_parcurs_B-151-VGT_iunie_2022_Alex_Bora.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
   <si>
     <t>VOLVO ROMÂNIA</t>
   </si>
@@ -70,40 +70,37 @@
     <t>Observatii utilizator</t>
   </si>
   <si>
+    <t>Acasa-Birou</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
     <t>Cluj-Apahida</t>
   </si>
   <si>
     <t>Interes Serviciu</t>
   </si>
   <si>
-    <t>Cluj-Cluj</t>
-  </si>
-  <si>
-    <t>Cluj-Bontida</t>
+    <t>Cluj-Satu-Mare</t>
+  </si>
+  <si>
+    <t>Cluj-Baia-Mare</t>
   </si>
   <si>
     <t>Cluj-Bistrita</t>
   </si>
   <si>
-    <t>Acasa-Birou</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Cluj-Satu-Mare</t>
+    <t>Cluj-Zalau</t>
+  </si>
+  <si>
+    <t>Cluj-Turda</t>
+  </si>
+  <si>
+    <t>Cluj-Dej</t>
   </si>
   <si>
     <t>Cluj-Cmp. Turzii</t>
-  </si>
-  <si>
-    <t>Cluj-Turda</t>
-  </si>
-  <si>
-    <t>Cluj-Baia-Mare</t>
-  </si>
-  <si>
-    <t>Cluj-Zalau</t>
   </si>
   <si>
     <t>Km parcursi:</t>
@@ -629,7 +626,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>307760</v>
+        <v>356153</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="20" customHeight="1">
@@ -661,7 +658,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="4">
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>17</v>
@@ -675,13 +672,13 @@
         <v>3</v>
       </c>
       <c r="B16" s="4">
-        <v>47</v>
+        <v>85</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="20" customHeight="1">
@@ -709,13 +706,13 @@
         <v>6</v>
       </c>
       <c r="B19" s="4">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="20" customHeight="1">
@@ -723,10 +720,10 @@
         <v>7</v>
       </c>
       <c r="B20" s="4">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>18</v>
@@ -737,10 +734,10 @@
         <v>8</v>
       </c>
       <c r="B21" s="4">
-        <v>257</v>
+        <v>30</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>18</v>
@@ -751,13 +748,13 @@
         <v>9</v>
       </c>
       <c r="B22" s="4">
-        <v>30</v>
+        <v>421</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="20" customHeight="1">
@@ -765,13 +762,13 @@
         <v>10</v>
       </c>
       <c r="B23" s="4">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="20" customHeight="1">
@@ -809,10 +806,10 @@
         <v>14</v>
       </c>
       <c r="B27" s="4">
-        <v>421</v>
+        <v>30</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>18</v>
@@ -823,10 +820,10 @@
         <v>15</v>
       </c>
       <c r="B28" s="4">
-        <v>152</v>
+        <v>30</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>18</v>
@@ -837,13 +834,13 @@
         <v>16</v>
       </c>
       <c r="B29" s="4">
-        <v>30</v>
+        <v>356</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="20" customHeight="1">
@@ -851,13 +848,13 @@
         <v>17</v>
       </c>
       <c r="B30" s="4">
-        <v>121</v>
+        <v>257</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="20" customHeight="1">
@@ -885,13 +882,13 @@
         <v>20</v>
       </c>
       <c r="B33" s="4">
-        <v>30</v>
+        <v>156</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="20" customHeight="1">
@@ -899,13 +896,13 @@
         <v>21</v>
       </c>
       <c r="B34" s="4">
-        <v>92</v>
+        <v>121</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="20" customHeight="1">
@@ -913,10 +910,10 @@
         <v>22</v>
       </c>
       <c r="B35" s="4">
-        <v>356</v>
+        <v>30</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>18</v>
@@ -927,10 +924,10 @@
         <v>23</v>
       </c>
       <c r="B36" s="4">
-        <v>156</v>
+        <v>30</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>18</v>
@@ -941,13 +938,13 @@
         <v>24</v>
       </c>
       <c r="B37" s="4">
-        <v>47</v>
+        <v>421</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="20" customHeight="1">
@@ -978,10 +975,10 @@
         <v>121</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="20" customHeight="1">
@@ -989,13 +986,13 @@
         <v>28</v>
       </c>
       <c r="B41" s="4">
-        <v>85</v>
+        <v>421</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="20" customHeight="1">
@@ -1003,13 +1000,13 @@
         <v>29</v>
       </c>
       <c r="B42" s="4">
-        <v>30</v>
+        <v>101</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="20" customHeight="1">
@@ -1017,59 +1014,59 @@
         <v>30</v>
       </c>
       <c r="B43" s="4">
-        <v>30</v>
+        <v>152</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="20" customHeight="1">
       <c r="A44" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B44" s="4">
-        <v>2259</v>
+        <v>2992</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="20" customHeight="1">
       <c r="A45" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B45" s="4">
-        <v>310019</v>
+        <v>359145</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="20" customHeight="1">
       <c r="A49" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="20" customHeight="1">
       <c r="A50" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="20" customHeight="1">
       <c r="A51" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="20" customHeight="1">
       <c r="A53" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="20" customHeight="1">
       <c r="A55" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="20" customHeight="1">
       <c r="A57" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
T460 -  duminică 10 iulie 2022, 18:01:03 +0300
</commit_message>
<xml_diff>
--- a/SCRATCH/CLEAN/foaie_parcurs_B-151-VGT_iunie_2022_Alex_Bora.xlsx
+++ b/SCRATCH/CLEAN/foaie_parcurs_B-151-VGT_iunie_2022_Alex_Bora.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="37">
   <si>
     <t>VOLVO ROMÂNIA</t>
   </si>
@@ -70,37 +70,40 @@
     <t>Observatii utilizator</t>
   </si>
   <si>
+    <t>Cluj-Apahida</t>
+  </si>
+  <si>
+    <t>Interes Serviciu</t>
+  </si>
+  <si>
+    <t>Cluj-Baia-Mare</t>
+  </si>
+  <si>
     <t>Acasa-Birou</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Cluj-Apahida</t>
-  </si>
-  <si>
-    <t>Interes Serviciu</t>
-  </si>
-  <si>
     <t>Cluj-Satu-Mare</t>
   </si>
   <si>
-    <t>Cluj-Baia-Mare</t>
+    <t>Cluj-Cmp. Turzii</t>
+  </si>
+  <si>
+    <t>Cluj-Turda</t>
+  </si>
+  <si>
+    <t>Cluj-Bontida</t>
+  </si>
+  <si>
+    <t>Cluj-Zalau</t>
   </si>
   <si>
     <t>Cluj-Bistrita</t>
   </si>
   <si>
-    <t>Cluj-Zalau</t>
-  </si>
-  <si>
-    <t>Cluj-Turda</t>
-  </si>
-  <si>
     <t>Cluj-Dej</t>
-  </si>
-  <si>
-    <t>Cluj-Cmp. Turzii</t>
   </si>
   <si>
     <t>Km parcursi:</t>
@@ -626,7 +629,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>356153</v>
+        <v>399863</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="20" customHeight="1">
@@ -658,7 +661,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="4">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>17</v>
@@ -672,13 +675,13 @@
         <v>3</v>
       </c>
       <c r="B16" s="4">
-        <v>85</v>
+        <v>356</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="20" customHeight="1">
@@ -706,13 +709,13 @@
         <v>6</v>
       </c>
       <c r="B19" s="4">
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="20" customHeight="1">
@@ -720,10 +723,10 @@
         <v>7</v>
       </c>
       <c r="B20" s="4">
-        <v>30</v>
+        <v>356</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>18</v>
@@ -734,10 +737,10 @@
         <v>8</v>
       </c>
       <c r="B21" s="4">
-        <v>30</v>
+        <v>421</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>18</v>
@@ -748,13 +751,13 @@
         <v>9</v>
       </c>
       <c r="B22" s="4">
-        <v>421</v>
+        <v>152</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="20" customHeight="1">
@@ -762,13 +765,13 @@
         <v>10</v>
       </c>
       <c r="B23" s="4">
-        <v>85</v>
+        <v>356</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="20" customHeight="1">
@@ -809,10 +812,10 @@
         <v>30</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="20" customHeight="1">
@@ -820,10 +823,10 @@
         <v>15</v>
       </c>
       <c r="B28" s="4">
-        <v>30</v>
+        <v>121</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>18</v>
@@ -834,13 +837,13 @@
         <v>16</v>
       </c>
       <c r="B29" s="4">
-        <v>356</v>
+        <v>92</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="20" customHeight="1">
@@ -848,13 +851,13 @@
         <v>17</v>
       </c>
       <c r="B30" s="4">
-        <v>257</v>
+        <v>156</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="20" customHeight="1">
@@ -882,13 +885,13 @@
         <v>20</v>
       </c>
       <c r="B33" s="4">
-        <v>156</v>
+        <v>30</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="20" customHeight="1">
@@ -896,13 +899,13 @@
         <v>21</v>
       </c>
       <c r="B34" s="4">
-        <v>121</v>
+        <v>30</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="20" customHeight="1">
@@ -910,10 +913,10 @@
         <v>22</v>
       </c>
       <c r="B35" s="4">
-        <v>30</v>
+        <v>257</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>18</v>
@@ -924,10 +927,10 @@
         <v>23</v>
       </c>
       <c r="B36" s="4">
-        <v>30</v>
+        <v>121</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>18</v>
@@ -938,13 +941,13 @@
         <v>24</v>
       </c>
       <c r="B37" s="4">
-        <v>421</v>
+        <v>30</v>
       </c>
       <c r="C37" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D37" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="20" customHeight="1">
@@ -972,13 +975,13 @@
         <v>27</v>
       </c>
       <c r="B40" s="4">
-        <v>121</v>
+        <v>30</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="20" customHeight="1">
@@ -986,13 +989,13 @@
         <v>28</v>
       </c>
       <c r="B41" s="4">
-        <v>421</v>
+        <v>30</v>
       </c>
       <c r="C41" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D41" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="20" customHeight="1">
@@ -1003,10 +1006,10 @@
         <v>101</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="20" customHeight="1">
@@ -1014,59 +1017,59 @@
         <v>30</v>
       </c>
       <c r="B43" s="4">
-        <v>152</v>
+        <v>92</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="20" customHeight="1">
       <c r="A44" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B44" s="4">
-        <v>2992</v>
+        <v>2876</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="20" customHeight="1">
       <c r="A45" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B45" s="4">
-        <v>359145</v>
+        <v>402739</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="20" customHeight="1">
       <c r="A49" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="20" customHeight="1">
       <c r="A50" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="20" customHeight="1">
       <c r="A51" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="20" customHeight="1">
       <c r="A53" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="20" customHeight="1">
       <c r="A55" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="20" customHeight="1">
       <c r="A57" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>